<commit_message>
Additional docuemnt wit hadded detail
</commit_message>
<xml_diff>
--- a/Documentation/MasterDocumentSummaryV1.xlsx
+++ b/Documentation/MasterDocumentSummaryV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50A4F69-DE89-4836-8CE1-F91378CE0D90}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508CDC9E-44C2-4D4A-878A-54A7DC522B7A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32325" yWindow="645" windowWidth="20070" windowHeight="13050" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="111">
   <si>
     <t>#</t>
   </si>
@@ -144,9 +144,6 @@
     <t xml:space="preserve">Courier parcel weights </t>
   </si>
   <si>
-    <t>To start</t>
-  </si>
-  <si>
     <t>Review Time</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>GRV, Supplier ctrl, prod ctrl</t>
   </si>
   <si>
-    <t>to start</t>
-  </si>
-  <si>
     <t>ReturnsToVendorVx</t>
   </si>
   <si>
@@ -355,6 +349,21 @@
   </si>
   <si>
     <t>Reduced content and hours</t>
+  </si>
+  <si>
+    <t>The appliation has been abandoned and hardware remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time adjusted from 16 hrs </t>
+  </si>
+  <si>
+    <t>reduced from 10 to 2 hours</t>
+  </si>
+  <si>
+    <t>ReceiveLabelJobsVx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job labellling measurements </t>
   </si>
 </sst>
 </file>
@@ -398,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -410,9 +419,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -729,11 +735,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D344755C-FC24-4480-8DDF-0AD33AAEB992}">
-  <dimension ref="A3:J62"/>
+  <dimension ref="A3:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,13 +777,13 @@
         <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>2</v>
@@ -785,26 +791,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="2">
         <v>12</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5">
+      <c r="G4" s="2">
         <v>2</v>
       </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
         <f t="shared" ref="I4:I5" si="0">G4+E4-H4</f>
         <v>14</v>
       </c>
@@ -812,26 +817,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="2">
         <v>12</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5">
+      <c r="G5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -860,7 +864,7 @@
         <v>19</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" ref="I6:I55" si="1">G6+E6-H6</f>
+        <f t="shared" ref="I6:I56" si="1">G6+E6-H6</f>
         <v>0</v>
       </c>
     </row>
@@ -951,7 +955,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" s="2">
         <v>1</v>
@@ -978,11 +982,11 @@
         <v>3</v>
       </c>
       <c r="H11" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>29</v>
@@ -1053,7 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1066,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1079,27 +1083,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="2" t="s">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="E22" s="2">
         <v>6</v>
@@ -1115,12 +1119,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E23" s="2">
         <v>4</v>
@@ -1136,12 +1140,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E24" s="2">
         <v>14</v>
@@ -1157,12 +1161,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>23</v>
@@ -1181,7 +1185,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1203,7 +1207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1216,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1229,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1242,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1255,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1263,7 +1267,7 @@
         <v>36</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E31" s="2">
         <v>3</v>
@@ -1272,19 +1276,22 @@
         <v>1</v>
       </c>
       <c r="H31" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D32" s="4">
         <v>0.9</v>
@@ -1296,22 +1303,22 @@
         <v>2</v>
       </c>
       <c r="H32" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="4">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="E33" s="2">
         <v>6</v>
@@ -1329,13 +1336,13 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="D34" s="4">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E34" s="2">
         <v>16</v>
@@ -1344,91 +1351,88 @@
         <v>2</v>
       </c>
       <c r="H34" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="E38" s="2">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G38" s="2">
         <v>2</v>
       </c>
       <c r="H38" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I38" s="2">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="E39" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G39" s="2">
         <v>1</v>
       </c>
       <c r="H39" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I39" s="2">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="E40" s="2">
         <v>9</v>
@@ -1446,13 +1450,10 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E41" s="2">
         <v>11</v>
@@ -1470,127 +1471,124 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" s="4">
-        <v>0.8</v>
+        <v>110</v>
       </c>
       <c r="E42" s="2">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G42" s="2">
+        <v>1</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
         <v>2</v>
-      </c>
-      <c r="H42" s="2">
-        <v>14</v>
-      </c>
-      <c r="I42" s="2">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D43" s="4">
         <v>0.8</v>
       </c>
       <c r="E43" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G43" s="2">
         <v>2</v>
       </c>
       <c r="H43" s="2">
+        <v>14</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E44" s="2">
+        <v>12</v>
+      </c>
+      <c r="G44" s="2">
+        <v>2</v>
+      </c>
+      <c r="H44" s="2">
         <v>9</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I44" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="J44" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C44" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="2">
-        <v>20</v>
-      </c>
-      <c r="G45" s="2">
-        <v>2</v>
-      </c>
-      <c r="H45" s="2">
-        <v>0</v>
-      </c>
-      <c r="I45" s="2">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E46" s="2">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G46" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H46" s="2">
         <v>0</v>
       </c>
       <c r="I46" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E47" s="2">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G47" s="2">
         <v>1</v>
@@ -1600,42 +1598,39 @@
       </c>
       <c r="I47" s="2">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E48" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G48" s="2">
         <v>1</v>
       </c>
       <c r="H48" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>23</v>
@@ -1654,114 +1649,117 @@
         <v>3</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E50" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G50" s="2">
         <v>1</v>
       </c>
       <c r="H50" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I50" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E51" s="2">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G51" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H51" s="2">
         <v>0</v>
       </c>
       <c r="I51" s="2">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E52" s="2">
         <v>30</v>
       </c>
       <c r="G52" s="2">
+        <v>3</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E53" s="2">
+        <v>30</v>
+      </c>
+      <c r="G53" s="2">
         <v>5</v>
       </c>
-      <c r="H52" s="2">
-        <v>0</v>
-      </c>
-      <c r="I52" s="2">
+      <c r="H53" s="2">
+        <v>0</v>
+      </c>
+      <c r="I53" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J52" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E53" s="2">
-        <v>6</v>
-      </c>
-      <c r="G53" s="2">
-        <v>1</v>
-      </c>
-      <c r="H53" s="2">
-        <v>0</v>
-      </c>
-      <c r="I53" s="2">
-        <f t="shared" si="1"/>
-        <v>7</v>
+      <c r="J53" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>23</v>
@@ -1782,10 +1780,10 @@
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>23</v>
@@ -1806,37 +1804,34 @@
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E56" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
       </c>
       <c r="I56" s="2">
-        <f t="shared" ref="I56" si="4">G56+E56-H56</f>
-        <v>0</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>94</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>23</v>
@@ -1851,25 +1846,52 @@
         <v>0</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" ref="I57" si="5">G57+E57-H57</f>
+        <f t="shared" ref="I57" si="4">G57+E57-H57</f>
         <v>0</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G62" s="2">
-        <f>SUM(G6:G61)</f>
-        <v>48</v>
-      </c>
-      <c r="H62" s="2">
-        <f>SUM(H6:H61)</f>
-        <v>126</v>
-      </c>
-      <c r="I62" s="2">
-        <f>SUM(I6:I61)-G62</f>
-        <v>238</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2">
+        <f t="shared" ref="I58" si="5">G58+E58-H58</f>
+        <v>0</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G63" s="2">
+        <f>SUM(G6:G62)</f>
+        <v>49</v>
+      </c>
+      <c r="H63" s="2">
+        <f>SUM(H6:H62)</f>
+        <v>140</v>
+      </c>
+      <c r="I63" s="2">
+        <f>SUM(I6:I62)-G63</f>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress and time spent update
</commit_message>
<xml_diff>
--- a/Documentation/MasterDocumentSummaryV1.xlsx
+++ b/Documentation/MasterDocumentSummaryV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508CDC9E-44C2-4D4A-878A-54A7DC522B7A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902C347A-F3C5-4EF0-AD14-AD9B5EF7F00C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="112">
   <si>
     <t>#</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Claims on supplier tracking and payment release</t>
   </si>
   <si>
-    <t>Non trivial solution due to supplier settlement permutations</t>
-  </si>
-  <si>
     <t>Picking controls</t>
   </si>
   <si>
@@ -364,6 +361,13 @@
   </si>
   <si>
     <t xml:space="preserve">Job labellling measurements </t>
+  </si>
+  <si>
+    <t>Reduced time from 20 hours - completed basic overview narrative
+Non trivial solution due to supplier settlement permutations</t>
+  </si>
+  <si>
+    <t>Time reduced from 14 hours. Limited narative provided</t>
   </si>
 </sst>
 </file>
@@ -738,8 +742,8 @@
   <dimension ref="A3:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,10 +796,10 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>23</v>
@@ -818,10 +822,10 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>23</v>
@@ -1085,25 +1089,25 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="E22" s="2">
         <v>6</v>
@@ -1121,10 +1125,10 @@
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="E23" s="2">
         <v>4</v>
@@ -1142,10 +1146,10 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E24" s="2">
         <v>14</v>
@@ -1163,10 +1167,10 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>23</v>
@@ -1283,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -1363,19 +1367,19 @@
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37" s="4"/>
     </row>
@@ -1400,16 +1404,16 @@
         <v>2</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="E39" s="2">
         <v>2</v>
       </c>
@@ -1424,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
@@ -1471,10 +1475,10 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E42" s="2">
         <v>1</v>
@@ -1498,7 +1502,7 @@
         <v>53</v>
       </c>
       <c r="D43" s="4">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="E43" s="2">
         <v>18</v>
@@ -1507,11 +1511,11 @@
         <v>2</v>
       </c>
       <c r="H43" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I43" s="2">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>56</v>
@@ -1525,7 +1529,7 @@
         <v>55</v>
       </c>
       <c r="D44" s="4">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="E44" s="2">
         <v>12</v>
@@ -1534,11 +1538,11 @@
         <v>2</v>
       </c>
       <c r="H44" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I44" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>56</v>
@@ -1546,7 +1550,7 @@
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D45" s="4"/>
     </row>
@@ -1557,56 +1561,53 @@
       <c r="C46" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E46" s="2">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G46" s="2">
         <v>2</v>
       </c>
       <c r="H46" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I46" s="2">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>59</v>
+        <v>2</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E47" s="2">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G47" s="2">
         <v>1</v>
       </c>
       <c r="H47" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I47" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>23</v>
@@ -1627,10 +1628,10 @@
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>23</v>
@@ -1649,15 +1650,15 @@
         <v>3</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>23</v>
@@ -1676,15 +1677,15 @@
         <v>3</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>23</v>
@@ -1705,10 +1706,10 @@
     </row>
     <row r="52" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>23</v>
@@ -1727,15 +1728,15 @@
         <v>33</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="E53" s="2">
         <v>30</v>
@@ -1751,15 +1752,15 @@
         <v>35</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>23</v>
@@ -1780,10 +1781,10 @@
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>23</v>
@@ -1804,10 +1805,10 @@
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>23</v>
@@ -1828,10 +1829,10 @@
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>23</v>
@@ -1850,15 +1851,15 @@
         <v>0</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>23</v>
@@ -1877,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
@@ -1887,11 +1888,11 @@
       </c>
       <c r="H63" s="2">
         <f>SUM(H6:H62)</f>
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="I63" s="2">
         <f>SUM(I6:I62)-G63</f>
-        <v>205</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the progress file
</commit_message>
<xml_diff>
--- a/Documentation/MasterDocumentSummaryV1.xlsx
+++ b/Documentation/MasterDocumentSummaryV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632F559E-4397-4E1A-9284-B463A6135C92}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2A1D98-554B-44F0-B6E9-67647EB9FD8F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
+    <workbookView xWindow="1275" yWindow="1800" windowWidth="21600" windowHeight="11835" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
   <si>
     <t>#</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t>Now forms part of Sage X3 largely</t>
+  </si>
+  <si>
+    <t>Tiem reduced from 8 hours</t>
   </si>
 </sst>
 </file>
@@ -773,9 +776,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D344755C-FC24-4480-8DDF-0AD33AAEB992}">
   <dimension ref="A3:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,21 +1663,24 @@
       <c r="C48" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>22</v>
+      <c r="D48" s="4">
+        <v>0.95</v>
       </c>
       <c r="E48" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G48" s="2">
         <v>1</v>
       </c>
       <c r="H48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -1946,11 +1952,11 @@
       </c>
       <c r="H64" s="2">
         <f>SUM(H6:H63)</f>
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I64" s="2">
         <f>SUM(I6:I63)-G64</f>
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added database diagrams and exe and proc names... and more stuff?
</commit_message>
<xml_diff>
--- a/Documentation/MasterDocumentSummaryV1.xlsx
+++ b/Documentation/MasterDocumentSummaryV1.xlsx
@@ -5,26 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B20F65E-ACFB-43A2-85FE-4048049AAD20}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9B1241-D357-4F39-8D2C-5FF222EC1F12}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -285,9 +279,6 @@
     <t>Debtors maintenance</t>
   </si>
   <si>
-    <t xml:space="preserve">X3 funcitonality </t>
-  </si>
-  <si>
     <t>Creditors maintenance</t>
   </si>
   <si>
@@ -392,6 +383,9 @@
   </si>
   <si>
     <t>SalOrderSplitV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X3 functionality </t>
   </si>
 </sst>
 </file>
@@ -792,8 +786,8 @@
   <dimension ref="A3:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -880,7 +874,7 @@
         <v>82</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -896,7 +890,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -973,7 +967,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>20</v>
@@ -995,7 +989,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1054,7 +1048,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" ref="H9:H30" si="2">G12+E12</f>
+        <f t="shared" ref="H12:H30" si="2">G12+E12</f>
         <v>0</v>
       </c>
       <c r="I12" s="2">
@@ -1142,25 +1136,25 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D22" s="4">
         <v>0.95</v>
@@ -1179,15 +1173,15 @@
         <v>1</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D23" s="4">
         <v>0.95</v>
@@ -1206,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1254,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -1355,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -1472,16 +1466,16 @@
         <v>2</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E39" s="2">
         <v>2</v>
       </c>
@@ -1496,7 +1490,7 @@
         <v>1</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
@@ -1523,7 +1517,7 @@
         <v>1</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1531,7 +1525,7 @@
         <v>47</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D41" s="4">
         <v>0.9</v>
@@ -1551,15 +1545,15 @@
         <v>1</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E42" s="2">
         <v>1</v>
@@ -1659,7 +1653,7 @@
         <v>2</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
@@ -1686,7 +1680,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
@@ -1713,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -1740,7 +1734,7 @@
         <v>3</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -1767,7 +1761,7 @@
         <v>3</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -1847,7 +1841,7 @@
     </row>
     <row r="54" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C54" s="7"/>
       <c r="J54" s="7"/>
@@ -1857,7 +1851,7 @@
         <v>83</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>21</v>
@@ -1878,10 +1872,10 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>21</v>
@@ -1902,10 +1896,10 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>21</v>
@@ -1926,10 +1920,10 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>21</v>
@@ -1948,15 +1942,15 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>21</v>
@@ -1975,7 +1969,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated status for indentShipping
</commit_message>
<xml_diff>
--- a/Documentation/MasterDocumentSummaryV1.xlsx
+++ b/Documentation/MasterDocumentSummaryV1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85871FB-2840-4896-8308-C72A836E6E45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5665049-9F88-4BE0-819B-382BD1596147}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
   </bookViews>
@@ -795,8 +795,8 @@
   <dimension ref="A3:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1166,7 @@
         <v>93</v>
       </c>
       <c r="D22" s="4">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
@@ -1175,11 +1175,11 @@
         <v>1</v>
       </c>
       <c r="H22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" ref="I22:I24" si="3">G22+E22-H22</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>116</v>
@@ -1994,11 +1994,11 @@
       </c>
       <c r="H64" s="2">
         <f>SUM(H6:H63)</f>
-        <v>163.5</v>
+        <v>164.5</v>
       </c>
       <c r="I64" s="2">
         <f>SUM(I6:I63)-G64</f>
-        <v>92.5</v>
+        <v>91.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Partial update while my machine is locked.
</commit_message>
<xml_diff>
--- a/Documentation/MasterDocumentSummaryV1.xlsx
+++ b/Documentation/MasterDocumentSummaryV1.xlsx
@@ -5,26 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85871FB-2840-4896-8308-C72A836E6E45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48D1416-5D2E-4B63-B3B9-5B12178E2961}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -51,9 +45,6 @@
     <t>Catalogue Lookup</t>
   </si>
   <si>
-    <t>System Funtion</t>
-  </si>
-  <si>
     <t>SalesDecisionSupportVx</t>
   </si>
   <si>
@@ -261,9 +252,6 @@
     <t>SundryVx</t>
   </si>
   <si>
-    <t xml:space="preserve">Provision for unknown programs &amp; funcitons </t>
-  </si>
-  <si>
     <t xml:space="preserve">Due to a period of time where funcitonality was enhanced outside of a controlled senvironment, the extent of funcitonality is not exact and provided for here, A visit with each user is required to determine the full extent </t>
   </si>
   <si>
@@ -340,9 +328,6 @@
   </si>
   <si>
     <t>ReceiveLabelJobsVx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Job labellling measurements </t>
   </si>
   <si>
     <t>Reduced time from 20 hours - completed basic overview narrative
@@ -395,6 +380,15 @@
   </si>
   <si>
     <t>Reduced time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job labelling measurements </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provision for unknown programs &amp; functions </t>
+  </si>
+  <si>
+    <t>System Function</t>
   </si>
 </sst>
 </file>
@@ -794,9 +788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D344755C-FC24-4480-8DDF-0AD33AAEB992}">
   <dimension ref="A3:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,25 +816,25 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>2</v>
@@ -849,10 +843,10 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -871,19 +865,19 @@
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -899,12 +893,12 @@
         <v>4</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -928,10 +922,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -952,10 +946,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -976,10 +970,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -998,15 +992,15 @@
         <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -1015,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="2">
         <v>1</v>
@@ -1030,7 +1024,7 @@
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -1049,12 +1043,12 @@
         <v>2</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" ref="H12:H30" si="2">G12+E12</f>
@@ -1067,7 +1061,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="2"/>
@@ -1080,7 +1074,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="2"/>
@@ -1093,7 +1087,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="2"/>
@@ -1106,7 +1100,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="2"/>
@@ -1119,7 +1113,7 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="2"/>
@@ -1132,7 +1126,7 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
@@ -1145,28 +1139,28 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D22" s="4">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
@@ -1182,15 +1176,15 @@
         <v>1</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
@@ -1209,15 +1203,15 @@
         <v>0</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" s="4">
         <v>0.9</v>
@@ -1236,15 +1230,15 @@
         <v>1</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" s="4">
         <v>0.9</v>
@@ -1263,12 +1257,12 @@
         <v>1</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="4">
         <v>0.9</v>
@@ -1290,7 +1284,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="2"/>
@@ -1303,7 +1297,7 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="2"/>
@@ -1316,7 +1310,7 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" si="2"/>
@@ -1329,7 +1323,7 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="2"/>
@@ -1342,10 +1336,10 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D31" s="4">
         <v>1</v>
@@ -1364,15 +1358,15 @@
         <v>0</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D32" s="4">
         <v>0.9</v>
@@ -1393,10 +1387,10 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>
@@ -1417,10 +1411,10 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
@@ -1439,33 +1433,33 @@
         <v>0</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="E38" s="2">
         <v>4</v>
@@ -1481,15 +1475,15 @@
         <v>2</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E39" s="2">
         <v>2</v>
@@ -1505,15 +1499,15 @@
         <v>1</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D40" s="4">
         <v>0.9</v>
@@ -1532,15 +1526,15 @@
         <v>1</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D41" s="4">
         <v>0.9</v>
@@ -1560,15 +1554,15 @@
         <v>1</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E42" s="2">
         <v>1</v>
@@ -1586,10 +1580,10 @@
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D43" s="4">
         <v>0.95</v>
@@ -1608,15 +1602,15 @@
         <v>2</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D44" s="4">
         <v>0.95</v>
@@ -1635,21 +1629,21 @@
         <v>2</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C45" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="D46" s="4">
         <v>0.9</v>
@@ -1668,15 +1662,15 @@
         <v>2</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="D47" s="4">
         <v>0.95</v>
@@ -1695,15 +1689,15 @@
         <v>1</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="D48" s="4">
         <v>0.95</v>
@@ -1722,15 +1716,15 @@
         <v>1</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D49" s="4">
         <v>0.95</v>
@@ -1749,15 +1743,15 @@
         <v>3</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D50" s="4">
         <v>0.95</v>
@@ -1776,18 +1770,18 @@
         <v>3</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E51" s="2">
         <v>9</v>
@@ -1805,13 +1799,13 @@
     </row>
     <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E52" s="2">
         <v>30</v>
@@ -1827,15 +1821,15 @@
         <v>33</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="E53" s="2">
         <v>30</v>
@@ -1851,25 +1845,25 @@
         <v>35</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C54" s="7"/>
       <c r="J54" s="7"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E55" s="2">
         <v>6</v>
@@ -1887,13 +1881,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E56" s="2">
         <v>6</v>
@@ -1911,13 +1905,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E57" s="2">
         <v>6</v>
@@ -1935,13 +1929,13 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E58" s="2">
         <v>0</v>
@@ -1957,18 +1951,18 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
@@ -1984,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added file reviewing SVN ePart deployment at high level Updated spreadsheet
</commit_message>
<xml_diff>
--- a/Documentation/MasterDocumentSummaryV1.xlsx
+++ b/Documentation/MasterDocumentSummaryV1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5665049-9F88-4BE0-819B-382BD1596147}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3F1F50-A069-4B5B-9156-9C70C4A83D8C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="124">
   <si>
     <t>#</t>
   </si>
@@ -395,6 +395,15 @@
   </si>
   <si>
     <t>Reduced time</t>
+  </si>
+  <si>
+    <t>ePartVesioningOverviewVx</t>
+  </si>
+  <si>
+    <t>Overview of SVN source code repository</t>
+  </si>
+  <si>
+    <t>Reduced from 8 hours</t>
   </si>
 </sst>
 </file>
@@ -792,18 +801,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D344755C-FC24-4480-8DDF-0AD33AAEB992}">
-  <dimension ref="A3:J64"/>
+  <dimension ref="A3:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -867,7 +876,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I5" si="0">G4+E4-H4</f>
+        <f t="shared" ref="I4:I6" si="0">G4+E4-H4</f>
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -903,174 +912,189 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6" s="2">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" ref="I6:I57" si="1">G6+E6-H6</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>11</v>
-      </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" ref="I7:I58" si="1">G7+E7-H7</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G8" s="2">
         <v>1</v>
       </c>
       <c r="H8" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
         <v>4</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2</v>
-      </c>
-      <c r="I10" s="2">
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
+      <c r="I11" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
         <v>17</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
         <v>3</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H12" s="2">
         <v>18</v>
       </c>
-      <c r="I11" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="J11" s="3" t="s">
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" ref="H12:H30" si="2">G12+E12</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H13:H31" si="2">G13+E13</f>
         <v>0</v>
       </c>
       <c r="I13" s="2">
@@ -1080,7 +1104,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="2"/>
@@ -1093,7 +1117,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="2"/>
@@ -1106,7 +1130,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="2"/>
@@ -1119,7 +1143,7 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="2"/>
@@ -1132,7 +1156,7 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
@@ -1145,52 +1169,38 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
-        <v>89</v>
+        <v>15</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-      <c r="H22" s="2">
-        <v>2</v>
-      </c>
-      <c r="I22" s="2">
-        <f t="shared" ref="I22:I24" si="3">G22+E22-H22</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
@@ -1205,105 +1215,119 @@
         <v>2</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I23:I25" si="3">G23+E23-H23</f>
         <v>0</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="D24" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G24" s="2">
         <v>1</v>
       </c>
       <c r="H24" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D25" s="4">
         <v>0.9</v>
       </c>
       <c r="E25" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G25" s="2">
         <v>1</v>
       </c>
       <c r="H25" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>27</v>
+        <v>60</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D26" s="4">
         <v>0.9</v>
       </c>
       <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E27" s="2">
         <v>15</v>
       </c>
-      <c r="G26" s="2">
-        <v>2</v>
-      </c>
-      <c r="H26" s="2">
-        <f>E26*D26</f>
+      <c r="G27" s="2">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2">
+        <f>E27*D27</f>
         <v>13.5</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I27" s="2">
         <f t="shared" si="1"/>
         <v>3.5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="2"/>
@@ -1316,7 +1340,7 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" si="2"/>
@@ -1329,7 +1353,7 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="2"/>
@@ -1341,294 +1365,280 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="4">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2">
-        <v>3</v>
-      </c>
-      <c r="G31" s="2">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H31" s="2">
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D32" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E32" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G32" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="4">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E33" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G33" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H33" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2">
+        <v>4</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="4">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2">
         <v>12</v>
       </c>
-      <c r="G34" s="2">
-        <v>2</v>
-      </c>
-      <c r="H34" s="2">
+      <c r="G35" s="2">
+        <v>2</v>
+      </c>
+      <c r="H35" s="2">
         <v>14</v>
       </c>
-      <c r="I34" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="2" t="s">
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C35" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" s="2">
-        <v>4</v>
-      </c>
-      <c r="G38" s="2">
-        <v>2</v>
-      </c>
-      <c r="H38" s="2">
-        <v>4</v>
-      </c>
-      <c r="I38" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>100</v>
-      </c>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="E39" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G39" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H39" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I39" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2">
+        <v>2</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D40" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E40" s="2">
-        <v>3</v>
-      </c>
-      <c r="G40" s="2">
-        <v>1</v>
-      </c>
-      <c r="H40" s="2">
-        <v>3</v>
-      </c>
-      <c r="I40" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D41" s="4">
         <v>0.9</v>
       </c>
       <c r="E41" s="2">
-        <v>2</v>
-      </c>
-      <c r="F41" s="2"/>
+        <v>3</v>
+      </c>
       <c r="G41" s="2">
         <v>1</v>
       </c>
       <c r="H41" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I41" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J41" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2">
+        <v>1</v>
+      </c>
+      <c r="H42" s="2">
+        <v>2</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E42" s="2">
-        <v>1</v>
-      </c>
-      <c r="G42" s="2">
-        <v>1</v>
-      </c>
-      <c r="H42" s="2">
-        <v>0</v>
-      </c>
-      <c r="I42" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="4">
-        <v>0.95</v>
+        <v>103</v>
       </c>
       <c r="E43" s="2">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G43" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H43" s="2">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I43" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D44" s="4">
         <v>0.95</v>
       </c>
       <c r="E44" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G44" s="2">
         <v>2</v>
       </c>
       <c r="H44" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I44" s="2">
         <f t="shared" si="1"/>
@@ -1639,125 +1649,125 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C45" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="E45" s="2">
+        <v>12</v>
+      </c>
+      <c r="G45" s="2">
+        <v>2</v>
+      </c>
+      <c r="H45" s="2">
+        <v>12</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <v>0.9</v>
       </c>
-      <c r="E46" s="2">
-        <v>2</v>
-      </c>
-      <c r="G46" s="2">
-        <v>2</v>
-      </c>
-      <c r="H46" s="2">
-        <v>2</v>
-      </c>
-      <c r="I46" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="J46" s="3" t="s">
+      <c r="E47" s="2">
+        <v>2</v>
+      </c>
+      <c r="G47" s="2">
+        <v>2</v>
+      </c>
+      <c r="H47" s="2">
+        <v>2</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J47" s="3" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="E47" s="2">
-        <v>2</v>
-      </c>
-      <c r="G47" s="2">
-        <v>1</v>
-      </c>
-      <c r="H47" s="2">
-        <v>2</v>
-      </c>
-      <c r="I47" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D48" s="4">
         <v>0.95</v>
       </c>
       <c r="E48" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G48" s="2">
         <v>1</v>
       </c>
       <c r="H48" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D49" s="4">
         <v>0.95</v>
       </c>
       <c r="E49" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G49" s="2">
         <v>1</v>
       </c>
       <c r="H49" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D50" s="4">
         <v>0.95</v>
@@ -1781,116 +1791,119 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="E51" s="2">
+        <v>4</v>
+      </c>
+      <c r="G51" s="2">
+        <v>1</v>
+      </c>
+      <c r="H51" s="2">
+        <v>2</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E51" s="2">
-        <v>9</v>
-      </c>
-      <c r="G51" s="2">
-        <v>1</v>
-      </c>
-      <c r="H51" s="2">
-        <v>0</v>
-      </c>
-      <c r="I51" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E52" s="2">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G52" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H52" s="2">
         <v>0</v>
       </c>
       <c r="I52" s="2">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E53" s="2">
         <v>30</v>
       </c>
       <c r="G53" s="2">
+        <v>3</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54" s="2">
+        <v>30</v>
+      </c>
+      <c r="G54" s="2">
         <v>5</v>
       </c>
-      <c r="H53" s="2">
-        <v>0</v>
-      </c>
-      <c r="I53" s="2">
+      <c r="H54" s="2">
+        <v>0</v>
+      </c>
+      <c r="I54" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J53" s="3" t="s">
+      <c r="J54" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+    <row r="55" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="J54" s="7"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E55" s="2">
-        <v>6</v>
-      </c>
-      <c r="G55" s="2">
-        <v>1</v>
-      </c>
-      <c r="H55" s="2">
-        <v>0</v>
-      </c>
-      <c r="I55" s="2">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
+      <c r="C55" s="7"/>
+      <c r="J55" s="7"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>21</v>
@@ -1911,10 +1924,10 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>21</v>
@@ -1935,7 +1948,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>118</v>
@@ -1944,25 +1957,22 @@
         <v>21</v>
       </c>
       <c r="E58" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" s="2">
         <v>0</v>
       </c>
       <c r="I58" s="2">
-        <f t="shared" ref="I58" si="4">G58+E58-H58</f>
-        <v>0</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>85</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>118</v>
@@ -1980,24 +1990,51 @@
         <v>0</v>
       </c>
       <c r="I59" s="2">
-        <f t="shared" ref="I59" si="5">G59+E59-H59</f>
+        <f t="shared" ref="I59" si="4">G59+E59-H59</f>
         <v>0</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G64" s="2">
-        <f>SUM(G6:G63)</f>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0</v>
+      </c>
+      <c r="G60" s="2">
+        <v>0</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0</v>
+      </c>
+      <c r="I60" s="2">
+        <f t="shared" ref="I60" si="5">G60+E60-H60</f>
+        <v>0</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G65" s="2">
+        <f>SUM(G7:G64)</f>
         <v>49</v>
       </c>
-      <c r="H64" s="2">
-        <f>SUM(H6:H63)</f>
+      <c r="H65" s="2">
+        <f>SUM(H7:H64)</f>
         <v>164.5</v>
       </c>
-      <c r="I64" s="2">
-        <f>SUM(I6:I63)-G64</f>
+      <c r="I65" s="2">
+        <f>SUM(I7:I64)-G65</f>
         <v>91.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Udpated the spreadsheet progress and completed stock journals
</commit_message>
<xml_diff>
--- a/Documentation/MasterDocumentSummaryV1.xlsx
+++ b/Documentation/MasterDocumentSummaryV1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89EACB8-54C2-4ACC-92AB-1231857ADE8C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B556A7-0891-4E2B-B63D-F4DC63B5C854}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
   </bookViews>
@@ -813,8 +813,8 @@
   <dimension ref="A3:J66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1297,7 @@
         <v>61</v>
       </c>
       <c r="D26" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E26" s="2">
         <v>4</v>
@@ -1789,7 +1789,7 @@
         <v>65</v>
       </c>
       <c r="D50" s="4">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E50" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Add more documentation details
</commit_message>
<xml_diff>
--- a/Documentation/MasterDocumentSummaryV1.xlsx
+++ b/Documentation/MasterDocumentSummaryV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AC19F0-ED0E-484E-BAAC-7E5FD7A6E08E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B406861F-5A78-41ED-8C19-A9750CB715BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{67F94A63-E538-4C5B-9912-E3ECC60CA507}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="129">
   <si>
     <t>#</t>
   </si>
@@ -413,6 +413,12 @@
   </si>
   <si>
     <t>Time reduced from 8 hours</t>
+  </si>
+  <si>
+    <t>Process included in the receiving actions</t>
+  </si>
+  <si>
+    <t>Development WIP</t>
   </si>
 </sst>
 </file>
@@ -462,7 +468,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -503,6 +509,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -823,7 +832,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1342,7 @@
         <v>59</v>
       </c>
       <c r="D27" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
@@ -1608,7 +1617,7 @@
         <v>46</v>
       </c>
       <c r="D42" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E42" s="2">
         <v>3</v>
@@ -1635,7 +1644,7 @@
         <v>107</v>
       </c>
       <c r="D43" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E43" s="2">
         <v>2</v>
@@ -1655,25 +1664,31 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E44" s="2">
-        <v>1</v>
-      </c>
-      <c r="G44" s="2">
-        <v>1</v>
-      </c>
-      <c r="H44" s="2">
-        <v>0</v>
-      </c>
-      <c r="I44" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
+      <c r="D44" s="9">
+        <v>1</v>
+      </c>
+      <c r="E44" s="8">
+        <v>1</v>
+      </c>
+      <c r="G44" s="8">
+        <v>1</v>
+      </c>
+      <c r="H44" s="8">
+        <v>0</v>
+      </c>
+      <c r="I44" s="8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
@@ -1887,6 +1902,9 @@
       <c r="I53" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>